<commit_message>
before the big cut
</commit_message>
<xml_diff>
--- a/src/data-analysis/correlation_matrix.xlsx
+++ b/src/data-analysis/correlation_matrix.xlsx
@@ -969,16 +969,16 @@
         <v>0.137875985434386</v>
       </c>
       <c r="BD2" t="n">
-        <v>-0.0800779832071101</v>
+        <v>-0.0815970767542159</v>
       </c>
       <c r="BE2" t="n">
-        <v>0.113047537188238</v>
+        <v>0.165249337410324</v>
       </c>
       <c r="BF2" t="n">
         <v>0.0993369614643579</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.0423641960897966</v>
+        <v>0.0874737962028333</v>
       </c>
       <c r="BH2" t="n">
         <v>-0.0076821025466434</v>
@@ -1163,16 +1163,16 @@
         <v>0.0229423577082042</v>
       </c>
       <c r="BD3" t="n">
-        <v>-0.0192855049814542</v>
+        <v>-0.0186186079645357</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.0426436626880106</v>
+        <v>0.0496916741584023</v>
       </c>
       <c r="BF3" t="n">
         <v>0.0166618042636445</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.0838743950119648</v>
+        <v>0.032881256825909</v>
       </c>
       <c r="BH3" t="n">
         <v>0.0312241740294486</v>
@@ -1357,16 +1357,16 @@
         <v>0.0540983305332001</v>
       </c>
       <c r="BD4" t="n">
-        <v>-0.0503434530778943</v>
+        <v>-0.0507231433964967</v>
       </c>
       <c r="BE4" t="n">
-        <v>-0.0194237097304581</v>
+        <v>0.0102553690281266</v>
       </c>
       <c r="BF4" t="n">
         <v>0.071491186586885</v>
       </c>
       <c r="BG4" t="n">
-        <v>-0.0517030602929854</v>
+        <v>-0.0405773299208589</v>
       </c>
       <c r="BH4" t="n">
         <v>-0.00534175300295884</v>
@@ -1551,16 +1551,16 @@
         <v>0.0746596981555183</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.0156892956557692</v>
+        <v>0.017862864673496</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.0840213434254051</v>
+        <v>0.0321434762748109</v>
       </c>
       <c r="BF5" t="n">
         <v>0.0352843092202589</v>
       </c>
       <c r="BG5" t="n">
-        <v>-0.0210294887051596</v>
+        <v>-0.0159863452280206</v>
       </c>
       <c r="BH5" t="n">
         <v>-0.0207798619519225</v>
@@ -1745,16 +1745,16 @@
         <v>0.169625619541247</v>
       </c>
       <c r="BD6" t="n">
-        <v>-0.0535682069272108</v>
+        <v>-0.0535468343660235</v>
       </c>
       <c r="BE6" t="n">
-        <v>0.143886758430298</v>
+        <v>0.17908550999353</v>
       </c>
       <c r="BF6" t="n">
         <v>0.0832205081089564</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.159934617713835</v>
+        <v>0.17836880932055</v>
       </c>
       <c r="BH6" t="n">
         <v>0.0498309995374498</v>
@@ -1939,16 +1939,16 @@
         <v>0.0873815578629734</v>
       </c>
       <c r="BD7" t="n">
-        <v>-0.0713455751919094</v>
+        <v>-0.0701371172919768</v>
       </c>
       <c r="BE7" t="n">
-        <v>0.0664635170654345</v>
+        <v>0.0666879039282731</v>
       </c>
       <c r="BF7" t="n">
         <v>0.0623930877436146</v>
       </c>
       <c r="BG7" t="n">
-        <v>-0.0459823146767166</v>
+        <v>-0.0208956592176667</v>
       </c>
       <c r="BH7" t="n">
         <v>-0.0158110902357104</v>
@@ -2133,16 +2133,16 @@
         <v>0.0141906568658574</v>
       </c>
       <c r="BD8" t="n">
-        <v>-0.023689946021887</v>
+        <v>-0.024182628271796</v>
       </c>
       <c r="BE8" t="n">
-        <v>0.0160284473347426</v>
+        <v>0.00424177307803122</v>
       </c>
       <c r="BF8" t="n">
         <v>0.0354847765108242</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.00458013546649144</v>
+        <v>0.0381655450866203</v>
       </c>
       <c r="BH8" t="n">
         <v>-0.0255986996945114</v>
@@ -2327,16 +2327,16 @@
         <v>0.421302474563674</v>
       </c>
       <c r="BD9" t="n">
-        <v>-0.017635563255962</v>
+        <v>-0.0189567315924209</v>
       </c>
       <c r="BE9" t="n">
-        <v>0.3737794302033</v>
+        <v>0.513541502505785</v>
       </c>
       <c r="BF9" t="n">
         <v>0.231318170088232</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.366941341593005</v>
+        <v>0.497186684721357</v>
       </c>
       <c r="BH9" t="n">
         <v>0.0341327391948365</v>
@@ -2521,16 +2521,16 @@
         <v>-0.033800983695316</v>
       </c>
       <c r="BD10" t="n">
-        <v>-0.0274881634991844</v>
+        <v>-0.0257241274852399</v>
       </c>
       <c r="BE10" t="n">
-        <v>0.0174449895958821</v>
+        <v>0.0160038166853782</v>
       </c>
       <c r="BF10" t="n">
         <v>0.0303691838831025</v>
       </c>
       <c r="BG10" t="n">
-        <v>0.0672148866285752</v>
+        <v>0.0317563832660057</v>
       </c>
       <c r="BH10" t="n">
         <v>0.0180905750709349</v>
@@ -2715,16 +2715,16 @@
         <v>0.0608202345838477</v>
       </c>
       <c r="BD11" t="n">
-        <v>-0.031218093775849</v>
+        <v>-0.0259028484782118</v>
       </c>
       <c r="BE11" t="n">
-        <v>0.0883229563602466</v>
+        <v>0.149516997944516</v>
       </c>
       <c r="BF11" t="n">
         <v>0.0390970448079661</v>
       </c>
       <c r="BG11" t="n">
-        <v>0.159607443602933</v>
+        <v>0.203252410432417</v>
       </c>
       <c r="BH11" t="n">
         <v>0.0118318003249266</v>
@@ -2909,16 +2909,16 @@
         <v>0.219901399921655</v>
       </c>
       <c r="BD12" t="n">
-        <v>-0.0391094816272913</v>
+        <v>-0.0409263581216176</v>
       </c>
       <c r="BE12" t="n">
-        <v>0.199737900100673</v>
+        <v>0.273235736339217</v>
       </c>
       <c r="BF12" t="n">
         <v>0.092029989670455</v>
       </c>
       <c r="BG12" t="n">
-        <v>0.164308839721769</v>
+        <v>0.202914597981061</v>
       </c>
       <c r="BH12" t="n">
         <v>0.0247197752771512</v>
@@ -3103,16 +3103,16 @@
         <v>-0.162957901951598</v>
       </c>
       <c r="BD13" t="n">
-        <v>-0.0380271810265841</v>
+        <v>-0.0434297731830801</v>
       </c>
       <c r="BE13" t="n">
-        <v>-0.0828197466115645</v>
+        <v>-0.0650535767685765</v>
       </c>
       <c r="BF13" t="n">
         <v>-0.10972593669406</v>
       </c>
       <c r="BG13" t="n">
-        <v>-0.0299847793054935</v>
+        <v>0.022155506651934</v>
       </c>
       <c r="BH13" t="n">
         <v>0.0110596573474417</v>
@@ -3297,16 +3297,16 @@
         <v>0.0867819822070494</v>
       </c>
       <c r="BD14" t="n">
-        <v>0.0157212639833224</v>
+        <v>0.011661773568604</v>
       </c>
       <c r="BE14" t="n">
-        <v>0.112930686130161</v>
+        <v>0.142237426080236</v>
       </c>
       <c r="BF14" t="n">
         <v>-0.011414367578915</v>
       </c>
       <c r="BG14" t="n">
-        <v>0.0376874508690499</v>
+        <v>0.0767961452168854</v>
       </c>
       <c r="BH14" t="n">
         <v>-0.0320461085925667</v>
@@ -3491,16 +3491,16 @@
         <v>-0.0534453741352028</v>
       </c>
       <c r="BD15" t="n">
-        <v>0.0316518945367693</v>
+        <v>0.0345816552522119</v>
       </c>
       <c r="BE15" t="n">
-        <v>0.0191476585703043</v>
+        <v>-0.0115017199220809</v>
       </c>
       <c r="BF15" t="n">
         <v>0.052340122100477</v>
       </c>
       <c r="BG15" t="n">
-        <v>0.0043481495302103</v>
+        <v>0.0371341558447095</v>
       </c>
       <c r="BH15" t="n">
         <v>-0.00664539588613711</v>
@@ -3685,16 +3685,16 @@
         <v>0.0414008468395056</v>
       </c>
       <c r="BD16" t="n">
-        <v>-0.0431793041613997</v>
+        <v>-0.04391923078595</v>
       </c>
       <c r="BE16" t="n">
-        <v>-0.0525525505560899</v>
+        <v>-0.107085376854479</v>
       </c>
       <c r="BF16" t="n">
         <v>0.172774938052262</v>
       </c>
       <c r="BG16" t="n">
-        <v>-0.0767463718826513</v>
+        <v>-0.0937404729383046</v>
       </c>
       <c r="BH16" t="n">
         <v>0.00918872016523076</v>
@@ -3879,16 +3879,16 @@
         <v>-0.0207517621859407</v>
       </c>
       <c r="BD17" t="n">
-        <v>0.0102708385114928</v>
+        <v>0.00584100188224373</v>
       </c>
       <c r="BE17" t="n">
-        <v>-0.0190271761307026</v>
+        <v>-0.0403219567801703</v>
       </c>
       <c r="BF17" t="n">
         <v>-0.0427313126799453</v>
       </c>
       <c r="BG17" t="n">
-        <v>-0.0497248323070192</v>
+        <v>-0.0763349896066238</v>
       </c>
       <c r="BH17" t="n">
         <v>-0.00632348188500437</v>
@@ -4073,16 +4073,16 @@
         <v>-0.0392727914879882</v>
       </c>
       <c r="BD18" t="n">
-        <v>0.0449408260211664</v>
+        <v>0.0483302036468243</v>
       </c>
       <c r="BE18" t="n">
-        <v>-0.00738398173172927</v>
+        <v>-0.00531167395482208</v>
       </c>
       <c r="BF18" t="n">
         <v>0.0248155311435485</v>
       </c>
       <c r="BG18" t="n">
-        <v>-0.00907814217552582</v>
+        <v>-0.0177955722910324</v>
       </c>
       <c r="BH18" t="n">
         <v>-0.0496090986448354</v>
@@ -4267,16 +4267,16 @@
         <v>-0.0450312733283355</v>
       </c>
       <c r="BD19" t="n">
-        <v>0.00131321061293928</v>
+        <v>0.00250091320131895</v>
       </c>
       <c r="BE19" t="n">
-        <v>-0.0483370880713143</v>
+        <v>-0.064759010166003</v>
       </c>
       <c r="BF19" t="n">
         <v>-0.0389563437530846</v>
       </c>
       <c r="BG19" t="n">
-        <v>-0.0321035187100828</v>
+        <v>-0.0174713218481976</v>
       </c>
       <c r="BH19" t="n">
         <v>0.0545822767636786</v>
@@ -4461,16 +4461,16 @@
         <v>0.142056231643089</v>
       </c>
       <c r="BD20" t="n">
-        <v>-0.0138061686667568</v>
+        <v>-0.0118446151714502</v>
       </c>
       <c r="BE20" t="n">
-        <v>0.0761773457027174</v>
+        <v>0.143164947915539</v>
       </c>
       <c r="BF20" t="n">
         <v>0.0594504214265865</v>
       </c>
       <c r="BG20" t="n">
-        <v>0.117403648280611</v>
+        <v>0.136495372929268</v>
       </c>
       <c r="BH20" t="n">
         <v>0.070378421024804</v>
@@ -4655,16 +4655,16 @@
         <v>0.0928609869266745</v>
       </c>
       <c r="BD21" t="n">
-        <v>-0.062197721004324</v>
+        <v>-0.0629060075107809</v>
       </c>
       <c r="BE21" t="n">
-        <v>-0.0250693994764483</v>
+        <v>-0.0300284629489641</v>
       </c>
       <c r="BF21" t="n">
         <v>0.108568734832296</v>
       </c>
       <c r="BG21" t="n">
-        <v>-0.0547278941951301</v>
+        <v>-0.0665352478493855</v>
       </c>
       <c r="BH21" t="n">
         <v>-0.0421773459623207</v>
@@ -4849,16 +4849,16 @@
         <v>-0.0392292329915022</v>
       </c>
       <c r="BD22" t="n">
-        <v>-0.0305566628175612</v>
+        <v>-0.0297698467338653</v>
       </c>
       <c r="BE22" t="n">
-        <v>-0.0259524309117402</v>
+        <v>-0.0298426017430108</v>
       </c>
       <c r="BF22" t="n">
         <v>0.0393740718938474</v>
       </c>
       <c r="BG22" t="n">
-        <v>-0.0616507643594443</v>
+        <v>-0.0704832495107391</v>
       </c>
       <c r="BH22" t="n">
         <v>-0.00741051046187151</v>
@@ -5043,16 +5043,16 @@
         <v>0.0146835598328764</v>
       </c>
       <c r="BD23" t="n">
-        <v>-0.00924140058966017</v>
+        <v>-0.007162213691849</v>
       </c>
       <c r="BE23" t="n">
-        <v>0.00602360373603521</v>
+        <v>-0.0123095937513826</v>
       </c>
       <c r="BF23" t="n">
         <v>0.0081984341668169</v>
       </c>
       <c r="BG23" t="n">
-        <v>-0.0107099163087687</v>
+        <v>-0.0338312454517021</v>
       </c>
       <c r="BH23" t="n">
         <v>0.0393153700438877</v>
@@ -5237,16 +5237,16 @@
         <v>-0.00288999122120547</v>
       </c>
       <c r="BD24" t="n">
-        <v>0.0281633094076566</v>
+        <v>0.0222234772734855</v>
       </c>
       <c r="BE24" t="n">
-        <v>0.0108960045209926</v>
+        <v>0.0342124594926799</v>
       </c>
       <c r="BF24" t="n">
         <v>-0.00457612427354408</v>
       </c>
       <c r="BG24" t="n">
-        <v>-0.0740923946246297</v>
+        <v>-0.0564506363108629</v>
       </c>
       <c r="BH24" t="n">
         <v>0.00512266009606255</v>
@@ -5431,16 +5431,16 @@
         <v>0.0961916389431745</v>
       </c>
       <c r="BD25" t="n">
-        <v>0.0117302919548002</v>
+        <v>0.0142891715818727</v>
       </c>
       <c r="BE25" t="n">
-        <v>0.0673803438595503</v>
+        <v>0.0548773065115783</v>
       </c>
       <c r="BF25" t="n">
         <v>0.0347319214899691</v>
       </c>
       <c r="BG25" t="n">
-        <v>0.0278859735345931</v>
+        <v>0.0239597877069605</v>
       </c>
       <c r="BH25" t="n">
         <v>-0.0267021909604982</v>
@@ -5625,16 +5625,16 @@
         <v>0.0609482194848665</v>
       </c>
       <c r="BD26" t="n">
-        <v>-0.0257610871067756</v>
+        <v>-0.0247992312670315</v>
       </c>
       <c r="BE26" t="n">
-        <v>0.0145518741018037</v>
+        <v>0.000168368191933544</v>
       </c>
       <c r="BF26" t="n">
         <v>0.0518570259455531</v>
       </c>
       <c r="BG26" t="n">
-        <v>0.00358560772143745</v>
+        <v>-0.0128740377390088</v>
       </c>
       <c r="BH26" t="n">
         <v>-0.00470968220487934</v>
@@ -5819,16 +5819,16 @@
         <v>-0.0889243302256765</v>
       </c>
       <c r="BD27" t="n">
-        <v>0.0934636535722648</v>
+        <v>0.0978797012763013</v>
       </c>
       <c r="BE27" t="n">
-        <v>-0.0874886757643221</v>
+        <v>-0.122245098091112</v>
       </c>
       <c r="BF27" t="n">
         <v>-0.144152339174951</v>
       </c>
       <c r="BG27" t="n">
-        <v>-0.119459246039315</v>
+        <v>-0.225539401689815</v>
       </c>
       <c r="BH27" t="n">
         <v>-0.013894515597316</v>
@@ -6013,16 +6013,16 @@
         <v>-0.0366421783728769</v>
       </c>
       <c r="BD28" t="n">
-        <v>0.00765069236358767</v>
+        <v>-0.00193501398833409</v>
       </c>
       <c r="BE28" t="n">
-        <v>-0.0467879440948055</v>
+        <v>-0.058789548985022</v>
       </c>
       <c r="BF28" t="n">
         <v>0.0516265942727171</v>
       </c>
       <c r="BG28" t="n">
-        <v>-0.051114840943988</v>
+        <v>-0.0820952318435051</v>
       </c>
       <c r="BH28" t="n">
         <v>-0.0412195240467931</v>
@@ -6207,16 +6207,16 @@
         <v>-0.0193386708838405</v>
       </c>
       <c r="BD29" t="n">
-        <v>-0.0187044379237624</v>
+        <v>-0.0190934360477366</v>
       </c>
       <c r="BE29" t="n">
-        <v>-0.0215254742584383</v>
+        <v>-0.0475629187254445</v>
       </c>
       <c r="BF29" t="n">
         <v>-0.0787872009696955</v>
       </c>
       <c r="BG29" t="n">
-        <v>0.0203906686865227</v>
+        <v>-0.0105209246457623</v>
       </c>
       <c r="BH29" t="n">
         <v>-0.00902111291822553</v>
@@ -6401,16 +6401,16 @@
         <v>-0.0249151894295247</v>
       </c>
       <c r="BD30" t="n">
-        <v>-0.0251377918463601</v>
+        <v>-0.0256605850951571</v>
       </c>
       <c r="BE30" t="n">
-        <v>-0.00529487850138295</v>
+        <v>0.0221890701830614</v>
       </c>
       <c r="BF30" t="n">
         <v>-0.00432516144762759</v>
       </c>
       <c r="BG30" t="n">
-        <v>-0.0165203032880537</v>
+        <v>-0.00444304868370972</v>
       </c>
       <c r="BH30" t="n">
         <v>0.0146126181479856</v>
@@ -6595,16 +6595,16 @@
         <v>-0.287362519724087</v>
       </c>
       <c r="BD31" t="n">
-        <v>-0.0298537932532563</v>
+        <v>-0.0310769450908443</v>
       </c>
       <c r="BE31" t="n">
-        <v>-0.168457657198081</v>
+        <v>-0.297191217456505</v>
       </c>
       <c r="BF31" t="n">
         <v>-0.331279841260345</v>
       </c>
       <c r="BG31" t="n">
-        <v>-0.16835083815766</v>
+        <v>-0.297102574714874</v>
       </c>
       <c r="BH31" t="n">
         <v>0.00838878298197601</v>
@@ -6789,16 +6789,16 @@
         <v>-0.00408166995105595</v>
       </c>
       <c r="BD32" t="n">
-        <v>-0.0109301011974979</v>
+        <v>-0.00752399438476918</v>
       </c>
       <c r="BE32" t="n">
-        <v>-0.00522080734041011</v>
+        <v>0.0247811044403265</v>
       </c>
       <c r="BF32" t="n">
         <v>0.0539222241891469</v>
       </c>
       <c r="BG32" t="n">
-        <v>0.0177522074267693</v>
+        <v>0.00251942162480776</v>
       </c>
       <c r="BH32" t="n">
         <v>-0.0213082174838789</v>
@@ -6983,16 +6983,16 @@
         <v>0.0315349925314979</v>
       </c>
       <c r="BD33" t="n">
-        <v>-0.0100193910940072</v>
+        <v>-0.00425529709519031</v>
       </c>
       <c r="BE33" t="n">
-        <v>0.0756524182385109</v>
+        <v>0.0821673415039533</v>
       </c>
       <c r="BF33" t="n">
         <v>0.0522322214632399</v>
       </c>
       <c r="BG33" t="n">
-        <v>0.0220178632106272</v>
+        <v>0.0208774333939504</v>
       </c>
       <c r="BH33" t="n">
         <v>0.025934404182161</v>
@@ -7177,16 +7177,16 @@
         <v>0.028934049460696</v>
       </c>
       <c r="BD34" t="n">
-        <v>-0.000248960274737447</v>
+        <v>-0.00193712226420609</v>
       </c>
       <c r="BE34" t="n">
-        <v>0.0226282325470203</v>
+        <v>0.0207075178857933</v>
       </c>
       <c r="BF34" t="n">
         <v>0.0246039308936222</v>
       </c>
       <c r="BG34" t="n">
-        <v>0.0135756831794605</v>
+        <v>0.0030368184563422</v>
       </c>
       <c r="BH34" t="n">
         <v>0.0265584255710763</v>
@@ -7371,16 +7371,16 @@
         <v>-0.0280514726068045</v>
       </c>
       <c r="BD35" t="n">
-        <v>-0.0182444951260346</v>
+        <v>-0.0169958311798479</v>
       </c>
       <c r="BE35" t="n">
-        <v>-0.0293112565906812</v>
+        <v>-0.0200113992629862</v>
       </c>
       <c r="BF35" t="n">
         <v>-0.0916004915803677</v>
       </c>
       <c r="BG35" t="n">
-        <v>0.0146388532164418</v>
+        <v>0.00897676306445121</v>
       </c>
       <c r="BH35" t="n">
         <v>0.026284087491238</v>
@@ -7565,16 +7565,16 @@
         <v>-0.0294396098537675</v>
       </c>
       <c r="BD36" t="n">
-        <v>0.0411613746464676</v>
+        <v>0.0406952337746304</v>
       </c>
       <c r="BE36" t="n">
-        <v>0.000487570395979105</v>
+        <v>0.0096982974978049</v>
       </c>
       <c r="BF36" t="n">
         <v>-0.0592449829057624</v>
       </c>
       <c r="BG36" t="n">
-        <v>-0.025054020725661</v>
+        <v>-0.00966447756929682</v>
       </c>
       <c r="BH36" t="n">
         <v>0.00620447135102862</v>
@@ -7759,16 +7759,16 @@
         <v>0.0120317660927524</v>
       </c>
       <c r="BD37" t="n">
-        <v>0.00839986137930876</v>
+        <v>0.00500905659211497</v>
       </c>
       <c r="BE37" t="n">
-        <v>0.0284171152798443</v>
+        <v>0.0487496545911144</v>
       </c>
       <c r="BF37" t="n">
         <v>0.0171533049174283</v>
       </c>
       <c r="BG37" t="n">
-        <v>0.0345505577439702</v>
+        <v>0.0350466153952265</v>
       </c>
       <c r="BH37" t="n">
         <v>-0.0147416629360505</v>
@@ -7953,16 +7953,16 @@
         <v>-0.039614894122735</v>
       </c>
       <c r="BD38" t="n">
-        <v>-0.0286868007516743</v>
+        <v>-0.0278324429975013</v>
       </c>
       <c r="BE38" t="n">
-        <v>-0.00826513779897493</v>
+        <v>0.00938432824509241</v>
       </c>
       <c r="BF38" t="n">
         <v>-0.0332162145628474</v>
       </c>
       <c r="BG38" t="n">
-        <v>-0.0481964016092147</v>
+        <v>-0.0460973441121476</v>
       </c>
       <c r="BH38" t="n">
         <v>-0.00239577200199072</v>
@@ -8147,16 +8147,16 @@
         <v>-0.00103175805954659</v>
       </c>
       <c r="BD39" t="n">
-        <v>0.0220001916271516</v>
+        <v>0.0265678090373746</v>
       </c>
       <c r="BE39" t="n">
-        <v>-0.0224939828796514</v>
+        <v>-0.0100068210054846</v>
       </c>
       <c r="BF39" t="n">
         <v>-0.0349361053553695</v>
       </c>
       <c r="BG39" t="n">
-        <v>-0.00552076467495431</v>
+        <v>-0.015598928925219</v>
       </c>
       <c r="BH39" t="n">
         <v>0.0392716421620989</v>
@@ -8341,16 +8341,16 @@
         <v>0.0331278734877646</v>
       </c>
       <c r="BD40" t="n">
-        <v>0.0520297876231425</v>
+        <v>0.0507878162546683</v>
       </c>
       <c r="BE40" t="n">
-        <v>0.0311044534970305</v>
+        <v>0.0695165273059637</v>
       </c>
       <c r="BF40" t="n">
         <v>0.0404160913687626</v>
       </c>
       <c r="BG40" t="n">
-        <v>0.0285423699294922</v>
+        <v>0.0265314920157896</v>
       </c>
       <c r="BH40" t="n">
         <v>-0.0366197543182839</v>
@@ -8535,16 +8535,16 @@
         <v>-0.0155696656247805</v>
       </c>
       <c r="BD41" t="n">
-        <v>0.0762723429087501</v>
+        <v>0.0619361502123216</v>
       </c>
       <c r="BE41" t="n">
-        <v>-0.0390884810866461</v>
+        <v>-0.0344315990831005</v>
       </c>
       <c r="BF41" t="n">
         <v>0.0109976642447054</v>
       </c>
       <c r="BG41" t="n">
-        <v>0.00157213909657275</v>
+        <v>-0.00210415077773631</v>
       </c>
       <c r="BH41" t="n">
         <v>0.017952609046798</v>
@@ -8729,16 +8729,16 @@
         <v>-0.0376962161407531</v>
       </c>
       <c r="BD42" t="n">
-        <v>-0.0277284398617089</v>
+        <v>-0.0268391164540621</v>
       </c>
       <c r="BE42" t="n">
-        <v>-0.0140342440775318</v>
+        <v>-0.0148766792557329</v>
       </c>
       <c r="BF42" t="n">
         <v>0.0201417447913149</v>
       </c>
       <c r="BG42" t="n">
-        <v>0.0395252395906268</v>
+        <v>0.0394201964533627</v>
       </c>
       <c r="BH42" t="n">
         <v>-0.00982779267092721</v>
@@ -8923,16 +8923,16 @@
         <v>-0.0116816684242029</v>
       </c>
       <c r="BD43" t="n">
-        <v>0.0106194991332085</v>
+        <v>0.0146558164871193</v>
       </c>
       <c r="BE43" t="n">
-        <v>0.065840845843109</v>
+        <v>0.0252223908150813</v>
       </c>
       <c r="BF43" t="n">
         <v>0.0142811372353293</v>
       </c>
       <c r="BG43" t="n">
-        <v>-0.0118685994779832</v>
+        <v>-0.00326568815881023</v>
       </c>
       <c r="BH43" t="n">
         <v>0.0160875086846265</v>
@@ -9117,16 +9117,16 @@
         <v>0.0321053951182718</v>
       </c>
       <c r="BD44" t="n">
-        <v>0.0312652391969012</v>
+        <v>0.0306662372704808</v>
       </c>
       <c r="BE44" t="n">
-        <v>0.00520538581319887</v>
+        <v>0.0117586543151287</v>
       </c>
       <c r="BF44" t="n">
         <v>0.0223933520121224</v>
       </c>
       <c r="BG44" t="n">
-        <v>0.0220330605370664</v>
+        <v>0.0226834643653461</v>
       </c>
       <c r="BH44" t="n">
         <v>-0.00998048855203995</v>
@@ -9311,16 +9311,16 @@
         <v>-0.0266205058367996</v>
       </c>
       <c r="BD45" t="n">
-        <v>-0.00554942743138562</v>
+        <v>-0.00255531966768799</v>
       </c>
       <c r="BE45" t="n">
-        <v>0.0124323970785566</v>
+        <v>0.0111582597334922</v>
       </c>
       <c r="BF45" t="n">
         <v>-0.0312390232674739</v>
       </c>
       <c r="BG45" t="n">
-        <v>0.0207021285538026</v>
+        <v>0.014512935154284</v>
       </c>
       <c r="BH45" t="n">
         <v>0.0345868436376459</v>
@@ -9505,16 +9505,16 @@
         <v>-0.0127745010689289</v>
       </c>
       <c r="BD46" t="n">
-        <v>-0.0356892342036838</v>
+        <v>-0.034247965573222</v>
       </c>
       <c r="BE46" t="n">
-        <v>0.00600499736667211</v>
+        <v>0.00099108326994771</v>
       </c>
       <c r="BF46" t="n">
         <v>-0.0085390361080467</v>
       </c>
       <c r="BG46" t="n">
-        <v>-0.0425067848074314</v>
+        <v>-0.0341711670754734</v>
       </c>
       <c r="BH46" t="n">
         <v>-0.0104401320832526</v>
@@ -9699,16 +9699,16 @@
         <v>-0.0137124811060819</v>
       </c>
       <c r="BD47" t="n">
-        <v>-0.047414755855332</v>
+        <v>-0.0471995636773539</v>
       </c>
       <c r="BE47" t="n">
-        <v>-0.0144993005227064</v>
+        <v>-0.0356929882491673</v>
       </c>
       <c r="BF47" t="n">
         <v>0.0129466209786697</v>
       </c>
       <c r="BG47" t="n">
-        <v>-0.0269959904873914</v>
+        <v>0.00880797757002593</v>
       </c>
       <c r="BH47" t="n">
         <v>-0.0511507862638921</v>
@@ -9893,16 +9893,16 @@
         <v>-0.010106593781333</v>
       </c>
       <c r="BD48" t="n">
-        <v>0.00498749279934021</v>
+        <v>0.00876985468125415</v>
       </c>
       <c r="BE48" t="n">
-        <v>-0.0120254997973305</v>
+        <v>-0.0195307145827924</v>
       </c>
       <c r="BF48" t="n">
         <v>0.0252089064461956</v>
       </c>
       <c r="BG48" t="n">
-        <v>-0.0114238266025081</v>
+        <v>0.0142390532762665</v>
       </c>
       <c r="BH48" t="n">
         <v>-0.0121552130448257</v>
@@ -10087,16 +10087,16 @@
         <v>0.026158824972552</v>
       </c>
       <c r="BD49" t="n">
-        <v>-0.0276639684425525</v>
+        <v>-0.0255663326678785</v>
       </c>
       <c r="BE49" t="n">
-        <v>0.00325206212322645</v>
+        <v>-0.00390967167098499</v>
       </c>
       <c r="BF49" t="n">
         <v>-0.0102659987328325</v>
       </c>
       <c r="BG49" t="n">
-        <v>-0.0164670727604175</v>
+        <v>-0.0210068393566191</v>
       </c>
       <c r="BH49" t="n">
         <v>-0.0470544975472919</v>
@@ -10281,16 +10281,16 @@
         <v>0.0113560062833614</v>
       </c>
       <c r="BD50" t="n">
-        <v>-0.0192153461671959</v>
+        <v>-0.0171451545797522</v>
       </c>
       <c r="BE50" t="n">
-        <v>-0.0170860656281027</v>
+        <v>-0.00581224398146135</v>
       </c>
       <c r="BF50" t="n">
         <v>-0.00002717134526493</v>
       </c>
       <c r="BG50" t="n">
-        <v>-0.000482392845930761</v>
+        <v>0.036434301250348</v>
       </c>
       <c r="BH50" t="n">
         <v>0.0321418041725514</v>
@@ -10475,16 +10475,16 @@
         <v>0.0174971052658272</v>
       </c>
       <c r="BD51" t="n">
-        <v>-0.0463155408818929</v>
+        <v>-0.04727876996086</v>
       </c>
       <c r="BE51" t="n">
-        <v>-0.0232441113437187</v>
+        <v>-0.029810885853571</v>
       </c>
       <c r="BF51" t="n">
         <v>0.0305827082002919</v>
       </c>
       <c r="BG51" t="n">
-        <v>0.0181321832266963</v>
+        <v>0.00686723621846886</v>
       </c>
       <c r="BH51" t="n">
         <v>-0.0715990453579585</v>
@@ -10669,16 +10669,16 @@
         <v>-0.0180151802644772</v>
       </c>
       <c r="BD52" t="n">
-        <v>-0.0515944835716771</v>
+        <v>-0.0526674993660358</v>
       </c>
       <c r="BE52" t="n">
-        <v>-0.00202029497660733</v>
+        <v>0.0138650992017474</v>
       </c>
       <c r="BF52" t="n">
         <v>-0.00385519707176671</v>
       </c>
       <c r="BG52" t="n">
-        <v>0.0387424172973548</v>
+        <v>0.0216665507759565</v>
       </c>
       <c r="BH52" t="n">
         <v>0.104148440641103</v>
@@ -10863,16 +10863,16 @@
         <v>0.0477666568483869</v>
       </c>
       <c r="BD53" t="n">
-        <v>0.0141637904104522</v>
+        <v>0.0103695091538202</v>
       </c>
       <c r="BE53" t="n">
-        <v>0.0101035426548905</v>
+        <v>-0.00406277576546642</v>
       </c>
       <c r="BF53" t="n">
         <v>0.0329902434585293</v>
       </c>
       <c r="BG53" t="n">
-        <v>-0.0112876858028021</v>
+        <v>-0.0532643259540156</v>
       </c>
       <c r="BH53" t="n">
         <v>-0.0069600188263875</v>
@@ -11057,16 +11057,16 @@
         <v>0.0427261806388474</v>
       </c>
       <c r="BD54" t="n">
-        <v>0.0414868451255451</v>
+        <v>0.0417454475030125</v>
       </c>
       <c r="BE54" t="n">
-        <v>0.00551100073785739</v>
+        <v>-0.0124539147173424</v>
       </c>
       <c r="BF54" t="n">
         <v>0.0322422130283957</v>
       </c>
       <c r="BG54" t="n">
-        <v>0.0190183481250732</v>
+        <v>-0.0163774032099617</v>
       </c>
       <c r="BH54" t="n">
         <v>0.011389241193119</v>
@@ -11251,16 +11251,16 @@
         <v>0.806658234053584</v>
       </c>
       <c r="BD55" t="n">
-        <v>0.0223919383500378</v>
+        <v>0.00962069059365277</v>
       </c>
       <c r="BE55" t="n">
-        <v>0.373842252793559</v>
+        <v>0.514833470045644</v>
       </c>
       <c r="BF55" t="n">
         <v>0.528993247256201</v>
       </c>
       <c r="BG55" t="n">
-        <v>0.227732164181112</v>
+        <v>0.336456079049175</v>
       </c>
       <c r="BH55" t="n">
         <v>0.00588067845231847</v>
@@ -11445,16 +11445,16 @@
         <v>1</v>
       </c>
       <c r="BD56" t="n">
-        <v>0.026832552626935</v>
+        <v>0.0101144173803749</v>
       </c>
       <c r="BE56" t="n">
-        <v>0.394464097759565</v>
+        <v>0.500983550567692</v>
       </c>
       <c r="BF56" t="n">
         <v>0.46130023468248</v>
       </c>
       <c r="BG56" t="n">
-        <v>0.192163377766149</v>
+        <v>0.308221180622334</v>
       </c>
       <c r="BH56" t="n">
         <v>-0.0172539567288593</v>
@@ -11474,390 +11474,390 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>-0.0800779832071101</v>
+        <v>-0.0815970767542159</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.0192855049814542</v>
+        <v>-0.0186186079645357</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.0503434530778943</v>
+        <v>-0.0507231433964967</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0156892956557692</v>
+        <v>0.017862864673496</v>
       </c>
       <c r="E57" t="n">
-        <v>-0.0535682069272108</v>
+        <v>-0.0535468343660235</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.0713455751919094</v>
+        <v>-0.0701371172919768</v>
       </c>
       <c r="G57" t="n">
-        <v>-0.023689946021887</v>
+        <v>-0.024182628271796</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.017635563255962</v>
+        <v>-0.0189567315924209</v>
       </c>
       <c r="I57" t="n">
-        <v>-0.0274881634991844</v>
+        <v>-0.0257241274852399</v>
       </c>
       <c r="J57" t="n">
-        <v>-0.031218093775849</v>
+        <v>-0.0259028484782118</v>
       </c>
       <c r="K57" t="n">
-        <v>-0.0391094816272913</v>
+        <v>-0.0409263581216176</v>
       </c>
       <c r="L57" t="n">
-        <v>-0.0380271810265841</v>
+        <v>-0.0434297731830801</v>
       </c>
       <c r="M57" t="n">
-        <v>0.0157212639833224</v>
+        <v>0.011661773568604</v>
       </c>
       <c r="N57" t="n">
-        <v>0.0316518945367693</v>
+        <v>0.0345816552522119</v>
       </c>
       <c r="O57" t="n">
-        <v>-0.0431793041613997</v>
+        <v>-0.04391923078595</v>
       </c>
       <c r="P57" t="n">
-        <v>0.0102708385114928</v>
+        <v>0.00584100188224373</v>
       </c>
       <c r="Q57" t="n">
-        <v>0.0449408260211664</v>
+        <v>0.0483302036468243</v>
       </c>
       <c r="R57" t="n">
-        <v>0.00131321061293928</v>
+        <v>0.00250091320131895</v>
       </c>
       <c r="S57" t="n">
-        <v>-0.0138061686667568</v>
+        <v>-0.0118446151714502</v>
       </c>
       <c r="T57" t="n">
-        <v>-0.062197721004324</v>
+        <v>-0.0629060075107809</v>
       </c>
       <c r="U57" t="n">
-        <v>-0.0305566628175612</v>
+        <v>-0.0297698467338653</v>
       </c>
       <c r="V57" t="n">
-        <v>-0.00924140058966017</v>
+        <v>-0.007162213691849</v>
       </c>
       <c r="W57" t="n">
-        <v>0.0281633094076566</v>
+        <v>0.0222234772734855</v>
       </c>
       <c r="X57" t="n">
-        <v>0.0117302919548002</v>
+        <v>0.0142891715818727</v>
       </c>
       <c r="Y57" t="n">
-        <v>-0.0257610871067756</v>
+        <v>-0.0247992312670315</v>
       </c>
       <c r="Z57" t="n">
-        <v>0.0934636535722648</v>
+        <v>0.0978797012763013</v>
       </c>
       <c r="AA57" t="n">
-        <v>0.00765069236358767</v>
+        <v>-0.00193501398833409</v>
       </c>
       <c r="AB57" t="n">
-        <v>-0.0187044379237624</v>
+        <v>-0.0190934360477366</v>
       </c>
       <c r="AC57" t="n">
-        <v>-0.0251377918463601</v>
+        <v>-0.0256605850951571</v>
       </c>
       <c r="AD57" t="n">
-        <v>-0.0298537932532563</v>
+        <v>-0.0310769450908443</v>
       </c>
       <c r="AE57" t="n">
-        <v>-0.0109301011974979</v>
+        <v>-0.00752399438476918</v>
       </c>
       <c r="AF57" t="n">
-        <v>-0.0100193910940072</v>
+        <v>-0.00425529709519031</v>
       </c>
       <c r="AG57" t="n">
-        <v>-0.000248960274737447</v>
+        <v>-0.00193712226420609</v>
       </c>
       <c r="AH57" t="n">
-        <v>-0.0182444951260346</v>
+        <v>-0.0169958311798479</v>
       </c>
       <c r="AI57" t="n">
-        <v>0.0411613746464676</v>
+        <v>0.0406952337746304</v>
       </c>
       <c r="AJ57" t="n">
-        <v>0.00839986137930876</v>
+        <v>0.00500905659211497</v>
       </c>
       <c r="AK57" t="n">
-        <v>-0.0286868007516743</v>
+        <v>-0.0278324429975013</v>
       </c>
       <c r="AL57" t="n">
-        <v>0.0220001916271516</v>
+        <v>0.0265678090373746</v>
       </c>
       <c r="AM57" t="n">
-        <v>0.0520297876231425</v>
+        <v>0.0507878162546683</v>
       </c>
       <c r="AN57" t="n">
-        <v>0.0762723429087501</v>
+        <v>0.0619361502123216</v>
       </c>
       <c r="AO57" t="n">
-        <v>-0.0277284398617089</v>
+        <v>-0.0268391164540621</v>
       </c>
       <c r="AP57" t="n">
-        <v>0.0106194991332085</v>
+        <v>0.0146558164871193</v>
       </c>
       <c r="AQ57" t="n">
-        <v>0.0312652391969012</v>
+        <v>0.0306662372704808</v>
       </c>
       <c r="AR57" t="n">
-        <v>-0.00554942743138562</v>
+        <v>-0.00255531966768799</v>
       </c>
       <c r="AS57" t="n">
-        <v>-0.0356892342036838</v>
+        <v>-0.034247965573222</v>
       </c>
       <c r="AT57" t="n">
-        <v>-0.047414755855332</v>
+        <v>-0.0471995636773539</v>
       </c>
       <c r="AU57" t="n">
-        <v>0.00498749279934021</v>
+        <v>0.00876985468125415</v>
       </c>
       <c r="AV57" t="n">
-        <v>-0.0276639684425525</v>
+        <v>-0.0255663326678785</v>
       </c>
       <c r="AW57" t="n">
-        <v>-0.0192153461671959</v>
+        <v>-0.0171451545797522</v>
       </c>
       <c r="AX57" t="n">
-        <v>-0.0463155408818929</v>
+        <v>-0.04727876996086</v>
       </c>
       <c r="AY57" t="n">
-        <v>-0.0515944835716771</v>
+        <v>-0.0526674993660358</v>
       </c>
       <c r="AZ57" t="n">
-        <v>0.0141637904104522</v>
+        <v>0.0103695091538202</v>
       </c>
       <c r="BA57" t="n">
-        <v>0.0414868451255451</v>
+        <v>0.0417454475030125</v>
       </c>
       <c r="BB57" t="n">
-        <v>0.0223919383500378</v>
+        <v>0.00962069059365277</v>
       </c>
       <c r="BC57" t="n">
-        <v>0.026832552626935</v>
+        <v>0.0101144173803749</v>
       </c>
       <c r="BD57" t="n">
         <v>1</v>
       </c>
       <c r="BE57" t="n">
-        <v>-0.0171643511258121</v>
+        <v>-0.019501128661448</v>
       </c>
       <c r="BF57" t="n">
-        <v>-0.0225483750142383</v>
+        <v>-0.0300353124887455</v>
       </c>
       <c r="BG57" t="n">
-        <v>-0.00682424932180748</v>
+        <v>-0.0385164450186748</v>
       </c>
       <c r="BH57" t="n">
-        <v>0.0365160505668881</v>
+        <v>0.041906726739293</v>
       </c>
       <c r="BI57" t="n">
-        <v>0.00434704015153366</v>
+        <v>0.000964581746617242</v>
       </c>
       <c r="BJ57" t="n">
-        <v>-0.0427263648712261</v>
+        <v>-0.0483088290670988</v>
       </c>
       <c r="BK57" t="n">
-        <v>0.00189961298704576</v>
+        <v>0.00581413584660816</v>
       </c>
       <c r="BL57" t="n">
-        <v>0.0442074841797508</v>
+        <v>0.0395908495412799</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.113047537188238</v>
+        <v>0.165249337410324</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0426436626880106</v>
+        <v>0.0496916741584023</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.0194237097304581</v>
+        <v>0.0102553690281266</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0840213434254051</v>
+        <v>0.0321434762748109</v>
       </c>
       <c r="E58" t="n">
-        <v>0.143886758430298</v>
+        <v>0.17908550999353</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0664635170654345</v>
+        <v>0.0666879039282731</v>
       </c>
       <c r="G58" t="n">
-        <v>0.0160284473347426</v>
+        <v>0.00424177307803122</v>
       </c>
       <c r="H58" t="n">
-        <v>0.3737794302033</v>
+        <v>0.513541502505785</v>
       </c>
       <c r="I58" t="n">
-        <v>0.0174449895958821</v>
+        <v>0.0160038166853782</v>
       </c>
       <c r="J58" t="n">
-        <v>0.0883229563602466</v>
+        <v>0.149516997944516</v>
       </c>
       <c r="K58" t="n">
-        <v>0.199737900100673</v>
+        <v>0.273235736339217</v>
       </c>
       <c r="L58" t="n">
-        <v>-0.0828197466115645</v>
+        <v>-0.0650535767685765</v>
       </c>
       <c r="M58" t="n">
-        <v>0.112930686130161</v>
+        <v>0.142237426080236</v>
       </c>
       <c r="N58" t="n">
-        <v>0.0191476585703043</v>
+        <v>-0.0115017199220809</v>
       </c>
       <c r="O58" t="n">
-        <v>-0.0525525505560899</v>
+        <v>-0.107085376854479</v>
       </c>
       <c r="P58" t="n">
-        <v>-0.0190271761307026</v>
+        <v>-0.0403219567801703</v>
       </c>
       <c r="Q58" t="n">
-        <v>-0.00738398173172927</v>
+        <v>-0.00531167395482208</v>
       </c>
       <c r="R58" t="n">
-        <v>-0.0483370880713143</v>
+        <v>-0.064759010166003</v>
       </c>
       <c r="S58" t="n">
-        <v>0.0761773457027174</v>
+        <v>0.143164947915539</v>
       </c>
       <c r="T58" t="n">
-        <v>-0.0250693994764483</v>
+        <v>-0.0300284629489641</v>
       </c>
       <c r="U58" t="n">
-        <v>-0.0259524309117402</v>
+        <v>-0.0298426017430108</v>
       </c>
       <c r="V58" t="n">
-        <v>0.00602360373603521</v>
+        <v>-0.0123095937513826</v>
       </c>
       <c r="W58" t="n">
-        <v>0.0108960045209926</v>
+        <v>0.0342124594926799</v>
       </c>
       <c r="X58" t="n">
-        <v>0.0673803438595503</v>
+        <v>0.0548773065115783</v>
       </c>
       <c r="Y58" t="n">
-        <v>0.0145518741018037</v>
+        <v>0.000168368191933544</v>
       </c>
       <c r="Z58" t="n">
-        <v>-0.0874886757643221</v>
+        <v>-0.122245098091112</v>
       </c>
       <c r="AA58" t="n">
-        <v>-0.0467879440948055</v>
+        <v>-0.058789548985022</v>
       </c>
       <c r="AB58" t="n">
-        <v>-0.0215254742584383</v>
+        <v>-0.0475629187254445</v>
       </c>
       <c r="AC58" t="n">
-        <v>-0.00529487850138295</v>
+        <v>0.0221890701830614</v>
       </c>
       <c r="AD58" t="n">
-        <v>-0.168457657198081</v>
+        <v>-0.297191217456505</v>
       </c>
       <c r="AE58" t="n">
-        <v>-0.00522080734041011</v>
+        <v>0.0247811044403265</v>
       </c>
       <c r="AF58" t="n">
-        <v>0.0756524182385109</v>
+        <v>0.0821673415039533</v>
       </c>
       <c r="AG58" t="n">
-        <v>0.0226282325470203</v>
+        <v>0.0207075178857933</v>
       </c>
       <c r="AH58" t="n">
-        <v>-0.0293112565906812</v>
+        <v>-0.0200113992629862</v>
       </c>
       <c r="AI58" t="n">
-        <v>0.000487570395979105</v>
+        <v>0.0096982974978049</v>
       </c>
       <c r="AJ58" t="n">
-        <v>0.0284171152798443</v>
+        <v>0.0487496545911144</v>
       </c>
       <c r="AK58" t="n">
-        <v>-0.00826513779897493</v>
+        <v>0.00938432824509241</v>
       </c>
       <c r="AL58" t="n">
-        <v>-0.0224939828796514</v>
+        <v>-0.0100068210054846</v>
       </c>
       <c r="AM58" t="n">
-        <v>0.0311044534970305</v>
+        <v>0.0695165273059637</v>
       </c>
       <c r="AN58" t="n">
-        <v>-0.0390884810866461</v>
+        <v>-0.0344315990831005</v>
       </c>
       <c r="AO58" t="n">
-        <v>-0.0140342440775318</v>
+        <v>-0.0148766792557329</v>
       </c>
       <c r="AP58" t="n">
-        <v>0.065840845843109</v>
+        <v>0.0252223908150813</v>
       </c>
       <c r="AQ58" t="n">
-        <v>0.00520538581319887</v>
+        <v>0.0117586543151287</v>
       </c>
       <c r="AR58" t="n">
-        <v>0.0124323970785566</v>
+        <v>0.0111582597334922</v>
       </c>
       <c r="AS58" t="n">
-        <v>0.00600499736667211</v>
+        <v>0.00099108326994771</v>
       </c>
       <c r="AT58" t="n">
-        <v>-0.0144993005227064</v>
+        <v>-0.0356929882491673</v>
       </c>
       <c r="AU58" t="n">
-        <v>-0.0120254997973305</v>
+        <v>-0.0195307145827924</v>
       </c>
       <c r="AV58" t="n">
-        <v>0.00325206212322645</v>
+        <v>-0.00390967167098499</v>
       </c>
       <c r="AW58" t="n">
-        <v>-0.0170860656281027</v>
+        <v>-0.00581224398146135</v>
       </c>
       <c r="AX58" t="n">
-        <v>-0.0232441113437187</v>
+        <v>-0.029810885853571</v>
       </c>
       <c r="AY58" t="n">
-        <v>-0.00202029497660733</v>
+        <v>0.0138650992017474</v>
       </c>
       <c r="AZ58" t="n">
-        <v>0.0101035426548905</v>
+        <v>-0.00406277576546642</v>
       </c>
       <c r="BA58" t="n">
-        <v>0.00551100073785739</v>
+        <v>-0.0124539147173424</v>
       </c>
       <c r="BB58" t="n">
-        <v>0.373842252793559</v>
+        <v>0.514833470045644</v>
       </c>
       <c r="BC58" t="n">
-        <v>0.394464097759565</v>
+        <v>0.500983550567692</v>
       </c>
       <c r="BD58" t="n">
-        <v>-0.0171643511258121</v>
+        <v>-0.019501128661448</v>
       </c>
       <c r="BE58" t="n">
         <v>1</v>
       </c>
       <c r="BF58" t="n">
-        <v>0.194665619717417</v>
+        <v>0.28397514852663</v>
       </c>
       <c r="BG58" t="n">
-        <v>0.23482665566461</v>
+        <v>0.45558759562675</v>
       </c>
       <c r="BH58" t="n">
-        <v>-0.0566041082540634</v>
+        <v>-0.0472914871855824</v>
       </c>
       <c r="BI58" t="n">
-        <v>0.0593361418537467</v>
+        <v>0.0865327605422411</v>
       </c>
       <c r="BJ58" t="n">
-        <v>-0.0258589296723775</v>
+        <v>-0.0567088353344402</v>
       </c>
       <c r="BK58" t="n">
-        <v>0.0240752508924961</v>
+        <v>0.0174911960499733</v>
       </c>
       <c r="BL58" t="n">
-        <v>0.244557291345228</v>
+        <v>0.435303777568798</v>
       </c>
     </row>
     <row r="59">
@@ -12027,16 +12027,16 @@
         <v>0.46130023468248</v>
       </c>
       <c r="BD59" t="n">
-        <v>-0.0225483750142383</v>
+        <v>-0.0300353124887455</v>
       </c>
       <c r="BE59" t="n">
-        <v>0.194665619717417</v>
+        <v>0.28397514852663</v>
       </c>
       <c r="BF59" t="n">
         <v>1</v>
       </c>
       <c r="BG59" t="n">
-        <v>0.144792780853745</v>
+        <v>0.226848200589505</v>
       </c>
       <c r="BH59" t="n">
         <v>0.0328207949291626</v>
@@ -12056,196 +12056,196 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.0423641960897966</v>
+        <v>0.0874737962028333</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0838743950119648</v>
+        <v>0.032881256825909</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.0517030602929854</v>
+        <v>-0.0405773299208589</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.0210294887051596</v>
+        <v>-0.0159863452280206</v>
       </c>
       <c r="E60" t="n">
-        <v>0.159934617713835</v>
+        <v>0.17836880932055</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.0459823146767166</v>
+        <v>-0.0208956592176667</v>
       </c>
       <c r="G60" t="n">
-        <v>0.00458013546649144</v>
+        <v>0.0381655450866203</v>
       </c>
       <c r="H60" t="n">
-        <v>0.366941341593005</v>
+        <v>0.497186684721357</v>
       </c>
       <c r="I60" t="n">
-        <v>0.0672148866285752</v>
+        <v>0.0317563832660057</v>
       </c>
       <c r="J60" t="n">
-        <v>0.159607443602933</v>
+        <v>0.203252410432417</v>
       </c>
       <c r="K60" t="n">
-        <v>0.164308839721769</v>
+        <v>0.202914597981061</v>
       </c>
       <c r="L60" t="n">
-        <v>-0.0299847793054935</v>
+        <v>0.022155506651934</v>
       </c>
       <c r="M60" t="n">
-        <v>0.0376874508690499</v>
+        <v>0.0767961452168854</v>
       </c>
       <c r="N60" t="n">
-        <v>0.0043481495302103</v>
+        <v>0.0371341558447095</v>
       </c>
       <c r="O60" t="n">
-        <v>-0.0767463718826513</v>
+        <v>-0.0937404729383046</v>
       </c>
       <c r="P60" t="n">
-        <v>-0.0497248323070192</v>
+        <v>-0.0763349896066238</v>
       </c>
       <c r="Q60" t="n">
-        <v>-0.00907814217552582</v>
+        <v>-0.0177955722910324</v>
       </c>
       <c r="R60" t="n">
-        <v>-0.0321035187100828</v>
+        <v>-0.0174713218481976</v>
       </c>
       <c r="S60" t="n">
-        <v>0.117403648280611</v>
+        <v>0.136495372929268</v>
       </c>
       <c r="T60" t="n">
-        <v>-0.0547278941951301</v>
+        <v>-0.0665352478493855</v>
       </c>
       <c r="U60" t="n">
-        <v>-0.0616507643594443</v>
+        <v>-0.0704832495107391</v>
       </c>
       <c r="V60" t="n">
-        <v>-0.0107099163087687</v>
+        <v>-0.0338312454517021</v>
       </c>
       <c r="W60" t="n">
-        <v>-0.0740923946246297</v>
+        <v>-0.0564506363108629</v>
       </c>
       <c r="X60" t="n">
-        <v>0.0278859735345931</v>
+        <v>0.0239597877069605</v>
       </c>
       <c r="Y60" t="n">
-        <v>0.00358560772143745</v>
+        <v>-0.0128740377390088</v>
       </c>
       <c r="Z60" t="n">
-        <v>-0.119459246039315</v>
+        <v>-0.225539401689815</v>
       </c>
       <c r="AA60" t="n">
-        <v>-0.051114840943988</v>
+        <v>-0.0820952318435051</v>
       </c>
       <c r="AB60" t="n">
-        <v>0.0203906686865227</v>
+        <v>-0.0105209246457623</v>
       </c>
       <c r="AC60" t="n">
-        <v>-0.0165203032880537</v>
+        <v>-0.00444304868370972</v>
       </c>
       <c r="AD60" t="n">
-        <v>-0.16835083815766</v>
+        <v>-0.297102574714874</v>
       </c>
       <c r="AE60" t="n">
-        <v>0.0177522074267693</v>
+        <v>0.00251942162480776</v>
       </c>
       <c r="AF60" t="n">
-        <v>0.0220178632106272</v>
+        <v>0.0208774333939504</v>
       </c>
       <c r="AG60" t="n">
-        <v>0.0135756831794605</v>
+        <v>0.0030368184563422</v>
       </c>
       <c r="AH60" t="n">
-        <v>0.0146388532164418</v>
+        <v>0.00897676306445121</v>
       </c>
       <c r="AI60" t="n">
-        <v>-0.025054020725661</v>
+        <v>-0.00966447756929682</v>
       </c>
       <c r="AJ60" t="n">
-        <v>0.0345505577439702</v>
+        <v>0.0350466153952265</v>
       </c>
       <c r="AK60" t="n">
-        <v>-0.0481964016092147</v>
+        <v>-0.0460973441121476</v>
       </c>
       <c r="AL60" t="n">
-        <v>-0.00552076467495431</v>
+        <v>-0.015598928925219</v>
       </c>
       <c r="AM60" t="n">
-        <v>0.0285423699294922</v>
+        <v>0.0265314920157896</v>
       </c>
       <c r="AN60" t="n">
-        <v>0.00157213909657275</v>
+        <v>-0.00210415077773631</v>
       </c>
       <c r="AO60" t="n">
-        <v>0.0395252395906268</v>
+        <v>0.0394201964533627</v>
       </c>
       <c r="AP60" t="n">
-        <v>-0.0118685994779832</v>
+        <v>-0.00326568815881023</v>
       </c>
       <c r="AQ60" t="n">
-        <v>0.0220330605370664</v>
+        <v>0.0226834643653461</v>
       </c>
       <c r="AR60" t="n">
-        <v>0.0207021285538026</v>
+        <v>0.014512935154284</v>
       </c>
       <c r="AS60" t="n">
-        <v>-0.0425067848074314</v>
+        <v>-0.0341711670754734</v>
       </c>
       <c r="AT60" t="n">
-        <v>-0.0269959904873914</v>
+        <v>0.00880797757002593</v>
       </c>
       <c r="AU60" t="n">
-        <v>-0.0114238266025081</v>
+        <v>0.0142390532762665</v>
       </c>
       <c r="AV60" t="n">
-        <v>-0.0164670727604175</v>
+        <v>-0.0210068393566191</v>
       </c>
       <c r="AW60" t="n">
-        <v>-0.000482392845930761</v>
+        <v>0.036434301250348</v>
       </c>
       <c r="AX60" t="n">
-        <v>0.0181321832266963</v>
+        <v>0.00686723621846886</v>
       </c>
       <c r="AY60" t="n">
-        <v>0.0387424172973548</v>
+        <v>0.0216665507759565</v>
       </c>
       <c r="AZ60" t="n">
-        <v>-0.0112876858028021</v>
+        <v>-0.0532643259540156</v>
       </c>
       <c r="BA60" t="n">
-        <v>0.0190183481250732</v>
+        <v>-0.0163774032099617</v>
       </c>
       <c r="BB60" t="n">
-        <v>0.227732164181112</v>
+        <v>0.336456079049175</v>
       </c>
       <c r="BC60" t="n">
-        <v>0.192163377766149</v>
+        <v>0.308221180622334</v>
       </c>
       <c r="BD60" t="n">
-        <v>-0.00682424932180748</v>
+        <v>-0.0385164450186748</v>
       </c>
       <c r="BE60" t="n">
-        <v>0.23482665566461</v>
+        <v>0.45558759562675</v>
       </c>
       <c r="BF60" t="n">
-        <v>0.144792780853745</v>
+        <v>0.226848200589505</v>
       </c>
       <c r="BG60" t="n">
         <v>1</v>
       </c>
       <c r="BH60" t="n">
-        <v>-0.00644189781606515</v>
+        <v>-0.0230488227842616</v>
       </c>
       <c r="BI60" t="n">
-        <v>0.0530545121560984</v>
+        <v>0.0595540612916295</v>
       </c>
       <c r="BJ60" t="n">
-        <v>-0.0599440059878854</v>
+        <v>-0.0466643869656188</v>
       </c>
       <c r="BK60" t="n">
-        <v>0.0135325483407948</v>
+        <v>0.0100134096717428</v>
       </c>
       <c r="BL60" t="n">
-        <v>0.300146005253798</v>
+        <v>0.434323138750505</v>
       </c>
     </row>
     <row r="61">
@@ -12415,16 +12415,16 @@
         <v>-0.0172539567288593</v>
       </c>
       <c r="BD61" t="n">
-        <v>0.0365160505668881</v>
+        <v>0.041906726739293</v>
       </c>
       <c r="BE61" t="n">
-        <v>-0.0566041082540634</v>
+        <v>-0.0472914871855824</v>
       </c>
       <c r="BF61" t="n">
         <v>0.0328207949291626</v>
       </c>
       <c r="BG61" t="n">
-        <v>-0.00644189781606515</v>
+        <v>-0.0230488227842616</v>
       </c>
       <c r="BH61" t="n">
         <v>1</v>
@@ -12609,16 +12609,16 @@
         <v>0.0676586225196399</v>
       </c>
       <c r="BD62" t="n">
-        <v>0.00434704015153366</v>
+        <v>0.000964581746617242</v>
       </c>
       <c r="BE62" t="n">
-        <v>0.0593361418537467</v>
+        <v>0.0865327605422411</v>
       </c>
       <c r="BF62" t="n">
         <v>0.0294324449901683</v>
       </c>
       <c r="BG62" t="n">
-        <v>0.0530545121560984</v>
+        <v>0.0595540612916295</v>
       </c>
       <c r="BH62" t="n">
         <v>-0.363133669123218</v>
@@ -12803,16 +12803,16 @@
         <v>-0.0325502240426268</v>
       </c>
       <c r="BD63" t="n">
-        <v>-0.0427263648712261</v>
+        <v>-0.0483088290670988</v>
       </c>
       <c r="BE63" t="n">
-        <v>-0.0258589296723775</v>
+        <v>-0.0567088353344402</v>
       </c>
       <c r="BF63" t="n">
         <v>0.0210595600731558</v>
       </c>
       <c r="BG63" t="n">
-        <v>-0.0599440059878854</v>
+        <v>-0.0466643869656188</v>
       </c>
       <c r="BH63" t="n">
         <v>-0.351413318159329</v>
@@ -12997,16 +12997,16 @@
         <v>-0.0204145734367597</v>
       </c>
       <c r="BD64" t="n">
-        <v>0.00189961298704576</v>
+        <v>0.00581413584660816</v>
       </c>
       <c r="BE64" t="n">
-        <v>0.0240752508924961</v>
+        <v>0.0174911960499733</v>
       </c>
       <c r="BF64" t="n">
         <v>-0.0906003486628821</v>
       </c>
       <c r="BG64" t="n">
-        <v>0.0135325483407948</v>
+        <v>0.0100134096717428</v>
       </c>
       <c r="BH64" t="n">
         <v>-0.303682749185041</v>
@@ -13191,16 +13191,16 @@
         <v>0.319275636009444</v>
       </c>
       <c r="BD65" t="n">
-        <v>0.0442074841797508</v>
+        <v>0.0395908495412799</v>
       </c>
       <c r="BE65" t="n">
-        <v>0.244557291345228</v>
+        <v>0.435303777568798</v>
       </c>
       <c r="BF65" t="n">
         <v>0.201001058120864</v>
       </c>
       <c r="BG65" t="n">
-        <v>0.300146005253798</v>
+        <v>0.434323138750505</v>
       </c>
       <c r="BH65" t="n">
         <v>-0.00198361751332295</v>

</xml_diff>